<commit_message>
Document number text box not working, successfully uploaded documents, Refresh not working
</commit_message>
<xml_diff>
--- a/Base-Template.xlsx
+++ b/Base-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarrar\Desktop\Professional\DevOps\AmazonInvoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC7054F-C7A2-4F2D-949F-145F053EE91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A3A9F8-D5F7-4CA1-A105-416A15F90E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,6 +34,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
@@ -92,9 +114,6 @@
 0.7mil (12ft x 10ft) - 17 Micron Thick, Save Time Decorating - Dust Sheet for
 Painting and Plastic Sheeting for Building Work
 ASIN: B09HXC3NL8</t>
-  </si>
-  <si>
-    <t>Sub Total</t>
   </si>
   <si>
     <t>Shipping</t>
@@ -124,6 +143,9 @@
   </si>
   <si>
     <t>Caelum Star - Trademan Enterprise</t>
+  </si>
+  <si>
+    <t>Sub Total (VAT EXCLUSIVE)</t>
   </si>
 </sst>
 </file>
@@ -351,6 +373,10 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -362,10 +388,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,7 +693,7 @@
   <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="A18" sqref="A18:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -698,16 +720,16 @@
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="19"/>
       <c r="D5" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="19"/>
       <c r="H5" s="10"/>
@@ -716,14 +738,14 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="28"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
+      <c r="A6" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
       <c r="H6" s="1" t="s">
         <v>1</v>
       </c>
@@ -732,12 +754,12 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
       <c r="H7" s="1" t="s">
         <v>3</v>
       </c>
@@ -746,27 +768,27 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
       <c r="H8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I8" s="13">
         <f>I22</f>
-        <v>35.849999999999994</v>
+        <v>19.710656999999998</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="H9" s="1" t="s">
         <v>6</v>
       </c>
@@ -775,12 +797,12 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="H10" s="1" t="s">
         <v>8</v>
       </c>
@@ -789,12 +811,12 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="H11" s="1" t="s">
         <v>10</v>
       </c>
@@ -806,13 +828,13 @@
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="26"/>
       <c r="G14" s="2" t="s">
         <v>14</v>
       </c>
@@ -827,49 +849,49 @@
       <c r="A15" s="6">
         <v>1</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="26"/>
       <c r="G15" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H15" s="14">
-        <v>11.95</v>
+        <v>10.95</v>
       </c>
       <c r="I15" s="15">
         <f>G15*H15</f>
-        <v>35.849999999999994</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="26"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
       <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
       <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
@@ -879,13 +901,13 @@
       <c r="G18" s="21"/>
       <c r="H18" s="21"/>
       <c r="I18" s="16">
-        <f>SUM(I15:I17)</f>
-        <v>35.849999999999994</v>
+        <f>(I15+I20)/1.2</f>
+        <v>16.424999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -900,7 +922,7 @@
     </row>
     <row r="20" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="21"/>
@@ -909,13 +931,14 @@
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
       <c r="H20" s="21"/>
-      <c r="I20" s="16">
-        <v>0</v>
+      <c r="I20" s="16" cm="1">
+        <f t="array" ref="I20">_xlfn.IFS(G15=1, -I15*0, G15=2, -I15*0.1, G15=3,-I15*0.2)</f>
+        <v>-2.19</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
@@ -925,13 +948,13 @@
       <c r="G21" s="21"/>
       <c r="H21" s="21"/>
       <c r="I21" s="16">
-        <f>(I18+I20)*20%</f>
-        <v>7.169999999999999</v>
+        <f>(SUM(I19:I20)+I15)*0.1667</f>
+        <v>3.2856569999999992</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -941,8 +964,8 @@
       <c r="G22" s="21"/>
       <c r="H22" s="21"/>
       <c r="I22" s="17">
-        <f>SUM(I18:I20)</f>
-        <v>35.849999999999994</v>
+        <f>SUM(I21,I18)</f>
+        <v>19.710656999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>